<commit_message>
code ready up to element types
</commit_message>
<xml_diff>
--- a/Building Characteristics.xlsx
+++ b/Building Characteristics.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://renewev.sharepoint.com/sites/RenewEV/Shared Documents/design tools/RenewEV Heat Loss Methodology/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlie\Documents\GitHub\RenewEV-Heat-Loss-Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="328" documentId="8_{109A9AF1-57E9-40DB-B7CC-86613E88E48D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF54A7D5-A0EB-49D3-9B0C-7346DEA8A0F7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605659A6-A469-42D3-B973-5127367F4723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="3" xr2:uid="{F7AB01C9-9591-4175-8402-68F676A903F8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F7AB01C9-9591-4175-8402-68F676A903F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="154">
   <si>
     <t>Element_Code</t>
   </si>
@@ -461,6 +461,48 @@
   </si>
   <si>
     <t>UK Gov Jan 2022</t>
+  </si>
+  <si>
+    <t>W1</t>
+  </si>
+  <si>
+    <t>W2</t>
+  </si>
+  <si>
+    <t>W3</t>
+  </si>
+  <si>
+    <t>W4</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>Insulation</t>
+  </si>
+  <si>
+    <t>https://www.acoustic-supplies.com/absorption-coefficient-chart/</t>
+  </si>
+  <si>
+    <t>Absoprtion Coefficient</t>
+  </si>
+  <si>
+    <t>IR_Surf</t>
+  </si>
+  <si>
+    <t>number of indoor radiation surfaces</t>
+  </si>
+  <si>
+    <t>Specific_Heat</t>
+  </si>
+  <si>
+    <t>2000-01-03  12:00:00</t>
+  </si>
+  <si>
+    <t>2000-01-04  18:00:00</t>
   </si>
 </sst>
 </file>
@@ -535,7 +577,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="22" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -563,6 +604,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="22" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -878,10 +920,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6DA64AD-AA06-4F69-BB92-B7A97995746A}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1094,8 +1136,8 @@
       <c r="A19" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="5">
-        <v>36527.5</v>
+      <c r="B19" s="16" t="s">
+        <v>152</v>
       </c>
       <c r="C19" t="s">
         <v>56</v>
@@ -1105,8 +1147,8 @@
       <c r="A20" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="5">
-        <v>36529.75</v>
+      <c r="B20" s="16" t="s">
+        <v>153</v>
       </c>
       <c r="C20" t="s">
         <v>57</v>
@@ -1125,13 +1167,24 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
+        <v>149</v>
+      </c>
+      <c r="B22" s="2">
+        <v>7</v>
+      </c>
+      <c r="C22" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>114</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B23" s="2">
         <f>SUM(Elements!O:O)</f>
-        <v>0</v>
-      </c>
-      <c r="C22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1145,235 +1198,499 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{716C0F2C-B08A-4EA2-B90D-300B6914284F}">
   <dimension ref="A1:V7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V2" sqref="A2:V7"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.08984375" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7265625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="9.90625" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="12" width="10.90625" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.453125" style="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7" style="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.26953125" style="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.36328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.81640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="18" max="22" width="7.453125" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="9.90625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="10.90625" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.453125" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.36328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.81640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="22" width="7.453125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="T1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="U1" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="V1" s="7" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
-      <c r="T2" s="13"/>
-      <c r="U2" s="13"/>
-      <c r="V2" s="13"/>
+      <c r="A2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" s="12">
+        <v>250</v>
+      </c>
+      <c r="I2" s="12">
+        <v>100</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="N2" s="12">
+        <v>5</v>
+      </c>
+      <c r="O2" s="12">
+        <v>0</v>
+      </c>
+      <c r="P2" s="12">
+        <v>90</v>
+      </c>
+      <c r="Q2" s="12">
+        <v>0</v>
+      </c>
+      <c r="R2" s="12">
+        <v>1</v>
+      </c>
+      <c r="S2" s="12">
+        <v>1</v>
+      </c>
+      <c r="T2" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="U2" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="V2" s="12" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
-      <c r="T3" s="13"/>
-      <c r="U3" s="13"/>
-      <c r="V3" s="13"/>
+      <c r="A3" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H3" s="12">
+        <v>250</v>
+      </c>
+      <c r="I3" s="12">
+        <v>100</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="N3" s="12">
+        <v>5</v>
+      </c>
+      <c r="O3" s="12">
+        <v>0</v>
+      </c>
+      <c r="P3" s="12">
+        <v>90</v>
+      </c>
+      <c r="Q3" s="12">
+        <v>-90</v>
+      </c>
+      <c r="R3" s="12">
+        <v>1</v>
+      </c>
+      <c r="S3" s="12">
+        <v>1</v>
+      </c>
+      <c r="T3" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="U3" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="V3" s="12" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="13"/>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="13"/>
-      <c r="V4" s="13"/>
+      <c r="A4" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H4" s="12">
+        <v>250</v>
+      </c>
+      <c r="I4" s="12">
+        <v>100</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="N4" s="12">
+        <v>5</v>
+      </c>
+      <c r="O4" s="12">
+        <v>0</v>
+      </c>
+      <c r="P4" s="12">
+        <v>90</v>
+      </c>
+      <c r="Q4" s="12">
+        <v>90</v>
+      </c>
+      <c r="R4" s="12">
+        <v>1</v>
+      </c>
+      <c r="S4" s="12">
+        <v>1</v>
+      </c>
+      <c r="T4" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="U4" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="V4" s="12" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="13"/>
-      <c r="S5" s="13"/>
-      <c r="T5" s="13"/>
-      <c r="U5" s="13"/>
-      <c r="V5" s="13"/>
+      <c r="A5" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H5" s="12">
+        <v>250</v>
+      </c>
+      <c r="I5" s="12">
+        <v>100</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="N5" s="12">
+        <v>5</v>
+      </c>
+      <c r="O5" s="12">
+        <v>0</v>
+      </c>
+      <c r="P5" s="12">
+        <v>90</v>
+      </c>
+      <c r="Q5" s="12">
+        <v>180</v>
+      </c>
+      <c r="R5" s="12">
+        <v>1</v>
+      </c>
+      <c r="S5" s="12">
+        <v>1</v>
+      </c>
+      <c r="T5" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="U5" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="V5" s="12" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="13"/>
-      <c r="S6" s="13"/>
-      <c r="T6" s="13"/>
-      <c r="U6" s="13"/>
-      <c r="V6" s="13"/>
+      <c r="A6" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H6" s="12">
+        <v>100</v>
+      </c>
+      <c r="I6" s="12">
+        <v>300</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="M6" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="N6" s="12">
+        <v>10</v>
+      </c>
+      <c r="O6" s="12">
+        <v>0</v>
+      </c>
+      <c r="P6" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="12">
+        <v>0</v>
+      </c>
+      <c r="R6" s="12">
+        <v>1</v>
+      </c>
+      <c r="S6" s="12">
+        <v>1</v>
+      </c>
+      <c r="T6" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="U6" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="V6" s="12" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="13"/>
-      <c r="S7" s="13"/>
-      <c r="T7" s="13"/>
-      <c r="U7" s="13"/>
-      <c r="V7" s="13"/>
+      <c r="A7" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H7" s="12">
+        <v>400</v>
+      </c>
+      <c r="I7" s="12">
+        <v>150</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="N7" s="12">
+        <v>10</v>
+      </c>
+      <c r="O7" s="12">
+        <v>25</v>
+      </c>
+      <c r="P7" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="12">
+        <v>0</v>
+      </c>
+      <c r="R7" s="12">
+        <v>1</v>
+      </c>
+      <c r="S7" s="12">
+        <v>1</v>
+      </c>
+      <c r="T7" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="U7" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="V7" s="12" t="s">
+        <v>101</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1390,7 +1707,7 @@
           <x14:formula1>
             <xm:f>Materials!$A$2:$A$199</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:G1048576</xm:sqref>
+          <xm:sqref>E8:G1048576 E2:G2 C2:D1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1408,96 +1725,96 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.7265625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="10" width="9.1796875" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="10.1796875" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="9.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="10.1796875" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="5" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1508,48 +1825,48 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E133CB3B-E7EE-41DB-9199-C6DD65C24FA5}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.90625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.08984375" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.26953125" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7265625" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.81640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.7265625" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7265625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.81640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.7265625" style="8" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="D1" s="8" t="s">
+      <c r="C1" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>99</v>
       </c>
       <c r="L1" s="1" t="s">
@@ -1560,28 +1877,28 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="H2" s="9" t="s">
+      <c r="A2" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>101</v>
       </c>
       <c r="L2" t="s">
@@ -1592,28 +1909,28 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="8">
         <v>2300</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="8">
         <v>880</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="8">
         <v>1.4</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="8">
         <v>0.9</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="8">
         <v>0</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="8">
         <v>0.25</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="8">
         <v>0.75</v>
       </c>
       <c r="L3" t="s">
@@ -1624,28 +1941,28 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <v>2500</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="8">
         <v>750</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="8">
         <v>1.4</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="8">
         <v>0.9</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="8">
         <v>0.83</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="8">
         <v>0.1</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="8">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L4" t="s">
@@ -1656,42 +1973,66 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>1.2</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <v>1000</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <v>0.25719999999999998</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="8">
         <v>0</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="8">
         <v>1</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="8">
         <v>0</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="8">
         <v>0</v>
       </c>
       <c r="L5" t="s">
         <v>96</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="M5" s="9" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="B6" s="8">
+        <v>130</v>
+      </c>
+      <c r="C6" s="8">
+        <v>2100</v>
+      </c>
+      <c r="D6" s="8">
+        <v>3.9E-2</v>
+      </c>
+      <c r="E6" s="8">
+        <v>0.95</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0</v>
+      </c>
+      <c r="G6" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="H6" s="8">
+        <v>0.7</v>
+      </c>
       <c r="L6" t="s">
         <v>97</v>
       </c>
-      <c r="M6" s="10" t="s">
+      <c r="M6" s="9" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1699,7 +2040,7 @@
       <c r="L7" t="s">
         <v>98</v>
       </c>
-      <c r="M7" s="10" t="s">
+      <c r="M7" s="9" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1707,7 +2048,7 @@
       <c r="L8" t="s">
         <v>99</v>
       </c>
-      <c r="M8" s="10" t="s">
+      <c r="M8" s="9" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1720,8 +2061,16 @@
       <c r="L11" t="s">
         <v>111</v>
       </c>
-      <c r="M11" s="11" t="s">
+      <c r="M11" s="10" t="s">
         <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="L12" t="s">
+        <v>148</v>
+      </c>
+      <c r="M12" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1907,23 +2256,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="16" t="s">
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="15" t="s">
         <v>131</v>
       </c>
     </row>
@@ -1964,7 +2313,7 @@
       <c r="L2" t="s">
         <v>130</v>
       </c>
-      <c r="M2" s="16"/>
+      <c r="M2" s="15"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
@@ -2025,7 +2374,7 @@
       <c r="A2" t="s">
         <v>134</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="13">
         <v>0.21448999999999999</v>
       </c>
     </row>
@@ -2033,7 +2382,7 @@
       <c r="A3" t="s">
         <v>135</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="13">
         <v>0.24676999999999999</v>
       </c>
     </row>
@@ -2041,7 +2390,7 @@
       <c r="A4" t="s">
         <v>136</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="13">
         <v>0.21232999999999999</v>
       </c>
     </row>
@@ -2049,7 +2398,7 @@
       <c r="A5" t="s">
         <v>137</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="13">
         <v>0.18315999999999999</v>
       </c>
     </row>
@@ -2059,6 +2408,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005E6C8E2BBE97A449BF587258ABB90B5C" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e50336969d1f6026fdc030928552f636">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9da34839-94b1-4adb-9ce9-2bf1180dd981" xmlns:ns3="e21e7998-6f05-4771-9945-6b2b40d9b8dc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="609895644b08c4e71b20ec11bc598037" ns2:_="" ns3:_="">
     <xsd:import namespace="9da34839-94b1-4adb-9ce9-2bf1180dd981"/>
@@ -2281,22 +2645,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86AA0889-6486-4C22-A950-9F61B4B8A696}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFAA5CEA-80BB-497C-B05C-1589868B6D5D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BA27988-4BDC-4DBB-93DD-2B86C53BCFE0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2313,21 +2679,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFAA5CEA-80BB-497C-B05C-1589868B6D5D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86AA0889-6486-4C22-A950-9F61B4B8A696}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
code failing in solver during As matrix formation. Something is wrong with the assembly of the C matrix as it gives a capacity to each window, door or skylight node with the same size as capicity of the indoor air
</commit_message>
<xml_diff>
--- a/Building Characteristics.xlsx
+++ b/Building Characteristics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlie\Documents\GitHub\RenewEV-Heat-Loss-Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605659A6-A469-42D3-B973-5127367F4723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB18170A-6F5D-4527-A75D-B7A51F6057D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F7AB01C9-9591-4175-8402-68F676A903F8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{F7AB01C9-9591-4175-8402-68F676A903F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="160">
   <si>
     <t>Element_Code</t>
   </si>
@@ -232,21 +232,6 @@
     <t>Thickness_5</t>
   </si>
   <si>
-    <t>Window - SinG</t>
-  </si>
-  <si>
-    <t>Window - SecG</t>
-  </si>
-  <si>
-    <t>Window - DG</t>
-  </si>
-  <si>
-    <t>Window - TG</t>
-  </si>
-  <si>
-    <t>Door - Single</t>
-  </si>
-  <si>
     <t>Floor - 5 Layers</t>
   </si>
   <si>
@@ -463,15 +448,6 @@
     <t>UK Gov Jan 2022</t>
   </si>
   <si>
-    <t>W1</t>
-  </si>
-  <si>
-    <t>W2</t>
-  </si>
-  <si>
-    <t>W3</t>
-  </si>
-  <si>
     <t>W4</t>
   </si>
   <si>
@@ -503,6 +479,48 @@
   </si>
   <si>
     <t>2000-01-04  18:00:00</t>
+  </si>
+  <si>
+    <t>Win1</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>Door</t>
+  </si>
+  <si>
+    <t>Skylight</t>
+  </si>
+  <si>
+    <t>Window</t>
+  </si>
+  <si>
+    <t>Soil Density</t>
+  </si>
+  <si>
+    <t>density of soil under building (kg/m3)</t>
+  </si>
+  <si>
+    <t>Soil Heat Capacity</t>
+  </si>
+  <si>
+    <t>heat capacity of soil under building (J/kg*K)</t>
+  </si>
+  <si>
+    <t>Soil Temp Depth</t>
+  </si>
+  <si>
+    <t>depth of soil associated with ground temperture (m)</t>
+  </si>
+  <si>
+    <t>Soil Conductivity</t>
+  </si>
+  <si>
+    <t>conductivity of soil under building (W/mK)</t>
   </si>
 </sst>
 </file>
@@ -598,13 +616,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="22" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -920,10 +938,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6DA64AD-AA06-4F69-BB92-B7A97995746A}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1136,8 +1154,8 @@
       <c r="A19" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="16" t="s">
-        <v>152</v>
+      <c r="B19" s="14" t="s">
+        <v>144</v>
       </c>
       <c r="C19" t="s">
         <v>56</v>
@@ -1147,8 +1165,8 @@
       <c r="A20" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="16" t="s">
-        <v>153</v>
+      <c r="B20" s="14" t="s">
+        <v>145</v>
       </c>
       <c r="C20" t="s">
         <v>57</v>
@@ -1167,25 +1185,69 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B22" s="2">
         <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B23" s="2">
         <f>SUM(Elements!O:O)</f>
         <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>113</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>152</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1500</v>
+      </c>
+      <c r="C24" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>154</v>
+      </c>
+      <c r="B25" s="2">
+        <v>1900</v>
+      </c>
+      <c r="C25" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>158</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>156</v>
+      </c>
+      <c r="B27" s="2">
+        <v>10</v>
+      </c>
+      <c r="C27" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -1198,8 +1260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{716C0F2C-B08A-4EA2-B90D-300B6914284F}">
   <dimension ref="A1:V7"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1254,7 +1316,7 @@
         <v>62</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="N1" s="7" t="s">
         <v>8</v>
@@ -1278,51 +1340,51 @@
         <v>14</v>
       </c>
       <c r="U1" s="7" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="V1" s="7" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>83</v>
+        <v>151</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>146</v>
+        <v>96</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="H2" s="12">
-        <v>250</v>
-      </c>
-      <c r="I2" s="12">
-        <v>100</v>
+        <v>96</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>96</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
+      </c>
+      <c r="M2" s="12">
+        <v>2</v>
       </c>
       <c r="N2" s="12">
         <v>5</v>
@@ -1339,58 +1401,58 @@
       <c r="R2" s="12">
         <v>1</v>
       </c>
-      <c r="S2" s="12">
-        <v>1</v>
+      <c r="S2" s="12" t="s">
+        <v>96</v>
       </c>
       <c r="T2" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="U2" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="V2" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>83</v>
+        <v>149</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>146</v>
+        <v>96</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="H3" s="12">
-        <v>250</v>
-      </c>
-      <c r="I3" s="12">
-        <v>100</v>
+        <v>96</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>96</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="M3" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
+      </c>
+      <c r="M3" s="12">
+        <v>1.5</v>
       </c>
       <c r="N3" s="12">
         <v>5</v>
@@ -1407,58 +1469,58 @@
       <c r="R3" s="12">
         <v>1</v>
       </c>
-      <c r="S3" s="12">
-        <v>1</v>
+      <c r="S3" s="12" t="s">
+        <v>96</v>
       </c>
       <c r="T3" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="U3" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="V3" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>83</v>
+        <v>150</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>146</v>
+        <v>96</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="H4" s="12">
-        <v>250</v>
-      </c>
-      <c r="I4" s="12">
-        <v>100</v>
+        <v>96</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>96</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="M4" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
+      </c>
+      <c r="M4" s="12">
+        <v>1</v>
       </c>
       <c r="N4" s="12">
         <v>5</v>
@@ -1475,58 +1537,58 @@
       <c r="R4" s="12">
         <v>1</v>
       </c>
-      <c r="S4" s="12">
-        <v>1</v>
+      <c r="S4" s="12" t="s">
+        <v>96</v>
       </c>
       <c r="T4" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="U4" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="V4" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H5" s="12">
-        <v>250</v>
+        <v>50</v>
       </c>
       <c r="I5" s="12">
         <v>100</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="N5" s="12">
         <v>5</v>
@@ -1547,54 +1609,54 @@
         <v>1</v>
       </c>
       <c r="T5" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="U5" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="V5" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C6" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="H6" s="12">
+        <v>50</v>
+      </c>
+      <c r="I6" s="12">
         <v>100</v>
       </c>
-      <c r="D6" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="H6" s="12">
-        <v>100</v>
-      </c>
-      <c r="I6" s="12">
-        <v>300</v>
-      </c>
       <c r="J6" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="N6" s="12">
         <v>10</v>
@@ -1615,54 +1677,54 @@
         <v>1</v>
       </c>
       <c r="T6" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="U6" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="V6" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C7" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="H7" s="12">
+        <v>50</v>
+      </c>
+      <c r="I7" s="12">
         <v>100</v>
       </c>
-      <c r="D7" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="H7" s="12">
-        <v>400</v>
-      </c>
-      <c r="I7" s="12">
-        <v>150</v>
-      </c>
       <c r="J7" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L7" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="N7" s="12">
         <v>10</v>
@@ -1683,13 +1745,13 @@
         <v>1</v>
       </c>
       <c r="T7" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="U7" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="V7" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1732,43 +1794,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>122</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
@@ -1846,71 +1908,71 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>98</v>
-      </c>
       <c r="H1" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="L2" t="s">
+        <v>88</v>
+      </c>
+      <c r="M2" t="s">
         <v>101</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="L2" t="s">
-        <v>93</v>
-      </c>
-      <c r="M2" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B3" s="8">
         <v>2300</v>
@@ -1934,15 +1996,15 @@
         <v>0.75</v>
       </c>
       <c r="L3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="M3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B4" s="8">
         <v>2500</v>
@@ -1966,15 +2028,15 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L4" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="M4" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B5" s="8">
         <v>1.2</v>
@@ -1998,15 +2060,15 @@
         <v>0</v>
       </c>
       <c r="L5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B6" s="8">
         <v>130</v>
@@ -2030,47 +2092,47 @@
         <v>0.7</v>
       </c>
       <c r="L6" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="L7" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="L8" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="M8" s="9" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="L10" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="L11" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="M11" s="10" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="L12" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="M12" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2083,10 +2145,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13609CCC-BA72-4DF1-844A-507F100E80C1}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2096,108 +2158,108 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>64</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
@@ -2212,17 +2274,7 @@
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>77</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -2256,64 +2308,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="15" t="s">
-        <v>131</v>
+      <c r="A1" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="16" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="F2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="H2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="I2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="J2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="K2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="L2" t="s">
-        <v>130</v>
-      </c>
-      <c r="M2" s="15"/>
+        <v>125</v>
+      </c>
+      <c r="M2" s="16"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
@@ -2361,18 +2413,18 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" t="s">
         <v>133</v>
       </c>
-      <c r="B1" t="s">
-        <v>138</v>
-      </c>
       <c r="D1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B2" s="13">
         <v>0.21448999999999999</v>
@@ -2380,7 +2432,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B3" s="13">
         <v>0.24676999999999999</v>
@@ -2388,7 +2440,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B4" s="13">
         <v>0.21232999999999999</v>
@@ -2396,7 +2448,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B5" s="13">
         <v>0.18315999999999999</v>
@@ -2408,21 +2460,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005E6C8E2BBE97A449BF587258ABB90B5C" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e50336969d1f6026fdc030928552f636">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9da34839-94b1-4adb-9ce9-2bf1180dd981" xmlns:ns3="e21e7998-6f05-4771-9945-6b2b40d9b8dc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="609895644b08c4e71b20ec11bc598037" ns2:_="" ns3:_="">
     <xsd:import namespace="9da34839-94b1-4adb-9ce9-2bf1180dd981"/>
@@ -2645,24 +2682,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86AA0889-6486-4C22-A950-9F61B4B8A696}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFAA5CEA-80BB-497C-B05C-1589868B6D5D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BA27988-4BDC-4DBB-93DD-2B86C53BCFE0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2679,4 +2714,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFAA5CEA-80BB-497C-B05C-1589868B6D5D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86AA0889-6486-4C22-A950-9F61B4B8A696}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
code failing still failing solver. Adding in post solver analysis.
</commit_message>
<xml_diff>
--- a/Building Characteristics.xlsx
+++ b/Building Characteristics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlie\Documents\GitHub\RenewEV-Heat-Loss-Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB18170A-6F5D-4527-A75D-B7A51F6057D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{964D1A70-156F-43A2-A05B-A82F2E4C6EAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{F7AB01C9-9591-4175-8402-68F676A903F8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F7AB01C9-9591-4175-8402-68F676A903F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="4" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="CO2 Conversion Factors" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="156">
   <si>
     <t>Element_Code</t>
   </si>
@@ -133,9 +134,6 @@
     <t>Tisp</t>
   </si>
   <si>
-    <t>DeltaT</t>
-  </si>
-  <si>
     <t>DeltaBlind</t>
   </si>
   <si>
@@ -202,9 +200,6 @@
     <t>desired indoor temperature (C)</t>
   </si>
   <si>
-    <t>max temperature difference for cooling</t>
-  </si>
-  <si>
     <t>max temperature difference for blinds controller</t>
   </si>
   <si>
@@ -464,12 +459,6 @@
   </si>
   <si>
     <t>Absoprtion Coefficient</t>
-  </si>
-  <si>
-    <t>IR_Surf</t>
-  </si>
-  <si>
-    <t>number of indoor radiation surfaces</t>
   </si>
   <si>
     <t>Specific_Heat</t>
@@ -938,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6DA64AD-AA06-4F69-BB92-B7A97995746A}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -956,10 +945,10 @@
         <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -970,7 +959,7 @@
         <v>300</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -981,7 +970,7 @@
         <v>1E-3</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -992,7 +981,7 @@
         <v>10000</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -1003,7 +992,7 @@
         <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -1014,7 +1003,7 @@
         <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -1025,7 +1014,7 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -1037,7 +1026,7 @@
         <v>293.14999999999998</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -1048,7 +1037,7 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -1059,7 +1048,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -1070,7 +1059,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -1081,7 +1070,7 @@
         <v>0.2</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -1092,7 +1081,7 @@
         <v>51</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -1103,7 +1092,7 @@
         <v>100</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -1114,7 +1103,7 @@
         <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -1122,32 +1111,32 @@
         <v>30</v>
       </c>
       <c r="B16" s="2">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="2">
-        <v>2</v>
+      <c r="B17" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>41</v>
+      <c r="B18" s="14" t="s">
+        <v>140</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -1155,99 +1144,77 @@
         <v>33</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="14" t="s">
-        <v>145</v>
+      <c r="B20" s="2">
+        <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>107</v>
       </c>
       <c r="B21" s="2">
-        <v>10</v>
+        <f>SUM(Elements!O:O)</f>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="B22" s="2">
-        <v>7</v>
+        <v>1500</v>
       </c>
       <c r="C22" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>109</v>
+        <v>150</v>
       </c>
       <c r="B23" s="2">
-        <f>SUM(Elements!O:O)</f>
-        <v>25</v>
+        <v>1900</v>
       </c>
       <c r="C23" t="s">
-        <v>108</v>
+        <v>151</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B24" s="2">
-        <v>1500</v>
+        <v>0.3</v>
       </c>
       <c r="C24" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B25" s="2">
-        <v>1900</v>
+        <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>158</v>
-      </c>
-      <c r="B26" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="C26" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>156</v>
-      </c>
-      <c r="B27" s="2">
-        <v>10</v>
-      </c>
-      <c r="C27" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -1260,8 +1227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{716C0F2C-B08A-4EA2-B90D-300B6914284F}">
   <dimension ref="A1:V7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6:I6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1295,10 +1262,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>5</v>
@@ -1310,13 +1277,13 @@
         <v>7</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="N1" s="7" t="s">
         <v>8</v>
@@ -1340,48 +1307,48 @@
         <v>14</v>
       </c>
       <c r="U1" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="V1" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M2" s="12">
         <v>2</v>
@@ -1402,54 +1369,54 @@
         <v>1</v>
       </c>
       <c r="S2" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="T2" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="U2" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="V2" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M3" s="12">
         <v>1.5</v>
@@ -1470,54 +1437,54 @@
         <v>1</v>
       </c>
       <c r="S3" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="T3" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="U3" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="V3" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M4" s="12">
         <v>1</v>
@@ -1538,57 +1505,57 @@
         <v>1</v>
       </c>
       <c r="S4" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="T4" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="U4" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="V4" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H5" s="12">
-        <v>50</v>
+        <v>0.5</v>
       </c>
       <c r="I5" s="12">
-        <v>100</v>
+        <v>0.6</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N5" s="12">
         <v>5</v>
@@ -1609,54 +1576,54 @@
         <v>1</v>
       </c>
       <c r="T5" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="U5" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="V5" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>138</v>
-      </c>
       <c r="E6" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H6" s="12">
-        <v>50</v>
+        <v>0.5</v>
       </c>
       <c r="I6" s="12">
-        <v>100</v>
+        <v>0.6</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N6" s="12">
         <v>10</v>
@@ -1677,54 +1644,54 @@
         <v>1</v>
       </c>
       <c r="T6" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="U6" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="V6" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H7" s="12">
-        <v>50</v>
+        <v>0.5</v>
       </c>
       <c r="I7" s="12">
-        <v>100</v>
+        <v>0.6</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L7" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N7" s="12">
         <v>10</v>
@@ -1745,13 +1712,13 @@
         <v>1</v>
       </c>
       <c r="T7" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="U7" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="V7" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1794,43 +1761,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>120</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
@@ -1890,7 +1857,7 @@
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B1" sqref="B1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1908,71 +1875,71 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="G1" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>94</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="M2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B3" s="8">
         <v>2300</v>
@@ -1996,15 +1963,15 @@
         <v>0.75</v>
       </c>
       <c r="L3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="M3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B4" s="8">
         <v>2500</v>
@@ -2028,15 +1995,15 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="M4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B5" s="8">
         <v>1.2</v>
@@ -2060,15 +2027,15 @@
         <v>0</v>
       </c>
       <c r="L5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B6" s="8">
         <v>130</v>
@@ -2092,47 +2059,47 @@
         <v>0.7</v>
       </c>
       <c r="L6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="L7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="L8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="M8" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="L10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="L11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="M11" s="10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="L12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="M12" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2158,123 +2125,123 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -2309,11 +2276,11 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D1" s="15"/>
       <c r="E1" s="15"/>
@@ -2325,45 +2292,45 @@
       <c r="K1" s="15"/>
       <c r="L1" s="15"/>
       <c r="M1" s="16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="L2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="M2" s="16"/>
     </row>
@@ -2413,18 +2380,18 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B2" s="13">
         <v>0.21448999999999999</v>
@@ -2432,7 +2399,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B3" s="13">
         <v>0.24676999999999999</v>
@@ -2440,7 +2407,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B4" s="13">
         <v>0.21232999999999999</v>
@@ -2448,7 +2415,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B5" s="13">
         <v>0.18315999999999999</v>
@@ -2683,18 +2650,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2717,18 +2684,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFAA5CEA-80BB-497C-B05C-1589868B6D5D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86AA0889-6486-4C22-A950-9F61B4B8A696}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFAA5CEA-80BB-497C-B05C-1589868B6D5D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>